<commit_message>
feat(Absent): export excel absent
</commit_message>
<xml_diff>
--- a/src/storage/app/excel-exporter/templates/resignation_decision.xlsx
+++ b/src/storage/app/excel-exporter/templates/resignation_decision.xlsx
@@ -286,12 +286,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -386,7 +386,7 @@
   <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -394,7 +394,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.72"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="19.14"/>
@@ -539,37 +539,37 @@
       <c r="B7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="K7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="M7" s="10" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>